<commit_message>
Update ILogger of Serilog
</commit_message>
<xml_diff>
--- a/Works Done.xlsx
+++ b/Works Done.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anara\OneDrive\Desktop\Repositories\Projects4Azer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D48B8E7-DA1A-4E13-8AAC-29E1E005E7CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7754B15-F826-44F6-AD1F-4686F9C2573A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="46">
   <si>
     <t>BotName</t>
   </si>
@@ -172,6 +172,9 @@
   </si>
   <si>
     <t>Working</t>
+  </si>
+  <si>
+    <t>Qalib</t>
   </si>
 </sst>
 </file>
@@ -699,8 +702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U11" sqref="U11"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="U20" sqref="U20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -881,13 +884,13 @@
         <f t="shared" ref="P3:P29" si="4">IF(O3="+","Düzgündür","Bilinmir")</f>
         <v>Düzgündür</v>
       </c>
-      <c r="Q3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="R3" s="1"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="S3" s="6" t="str">
         <f t="shared" ref="S3:S29" si="5">IF(R3="+","Düzgündür","Bilinmir")</f>
-        <v>Bilinmir</v>
+        <v>Düzgündür</v>
       </c>
       <c r="T3" s="3" t="s">
         <v>21</v>
@@ -942,13 +945,13 @@
         <f t="shared" si="4"/>
         <v>Düzgündür</v>
       </c>
-      <c r="Q4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="R4" s="1"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="S4" s="6" t="str">
         <f t="shared" si="5"/>
-        <v>Bilinmir</v>
+        <v>Düzgündür</v>
       </c>
       <c r="T4" s="3" t="s">
         <v>13</v>
@@ -1003,13 +1006,13 @@
         <f t="shared" si="4"/>
         <v>Düzgündür</v>
       </c>
-      <c r="Q5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="R5" s="1"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="S5" s="6" t="str">
         <f t="shared" si="5"/>
-        <v>Bilinmir</v>
+        <v>Düzgündür</v>
       </c>
       <c r="T5" s="3" t="s">
         <v>13</v>
@@ -1064,13 +1067,13 @@
         <f t="shared" si="4"/>
         <v>Düzgündür</v>
       </c>
-      <c r="Q6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="R6" s="1"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="S6" s="6" t="str">
         <f t="shared" si="5"/>
-        <v>Bilinmir</v>
+        <v>Düzgündür</v>
       </c>
       <c r="T6" s="3" t="s">
         <v>13</v>
@@ -1122,10 +1125,12 @@
         <v>Bilinmir</v>
       </c>
       <c r="Q7" s="3"/>
-      <c r="R7" s="1"/>
+      <c r="R7" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="S7" s="6" t="str">
         <f t="shared" si="5"/>
-        <v>Bilinmir</v>
+        <v>Düzgündür</v>
       </c>
       <c r="T7" s="3" t="s">
         <v>21</v>
@@ -1179,12 +1184,14 @@
         <v>Düzgündür</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="R8" s="1"/>
+        <v>45</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="S8" s="6" t="str">
         <f t="shared" si="5"/>
-        <v>Bilinmir</v>
+        <v>Düzgündür</v>
       </c>
       <c r="T8" s="3" t="s">
         <v>13</v>
@@ -1239,13 +1246,13 @@
         <f t="shared" si="4"/>
         <v>Düzgündür</v>
       </c>
-      <c r="Q9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="R9" s="1"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="S9" s="6" t="str">
         <f t="shared" si="5"/>
-        <v>Bilinmir</v>
+        <v>Düzgündür</v>
       </c>
       <c r="T9" s="3" t="s">
         <v>13</v>
@@ -1300,13 +1307,13 @@
         <f t="shared" si="4"/>
         <v>Bilinmir</v>
       </c>
-      <c r="Q10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="R10" s="1"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="S10" s="6" t="str">
         <f t="shared" si="5"/>
-        <v>Bilinmir</v>
+        <v>Düzgündür</v>
       </c>
       <c r="T10" s="3" t="s">
         <v>13</v>
@@ -1361,13 +1368,13 @@
         <f t="shared" si="4"/>
         <v>Bilinmir</v>
       </c>
-      <c r="Q11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="R11" s="1"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="S11" s="6" t="str">
         <f t="shared" si="5"/>
-        <v>Bilinmir</v>
+        <v>Düzgündür</v>
       </c>
       <c r="T11" s="3" t="s">
         <v>13</v>
@@ -1422,9 +1429,7 @@
         <f t="shared" si="4"/>
         <v>Düzgündür</v>
       </c>
-      <c r="Q12" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="Q12" s="3"/>
       <c r="R12" s="1" t="s">
         <v>13</v>
       </c>
@@ -1487,9 +1492,7 @@
         <f t="shared" si="4"/>
         <v>Düzgündür</v>
       </c>
-      <c r="Q13" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="Q13" s="3"/>
       <c r="R13" s="1" t="s">
         <v>13</v>
       </c>
@@ -1550,10 +1553,10 @@
         <f t="shared" si="4"/>
         <v>Bilinmir</v>
       </c>
-      <c r="Q14" s="3" t="s">
+      <c r="Q14" s="3"/>
+      <c r="R14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="R14" s="1"/>
       <c r="S14" s="6" t="str">
         <f t="shared" si="5"/>
         <v>Bilinmir</v>
@@ -1611,13 +1614,13 @@
         <f t="shared" si="4"/>
         <v>Düzgündür</v>
       </c>
-      <c r="Q15" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="R15" s="1"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="S15" s="6" t="str">
         <f t="shared" si="5"/>
-        <v>Bilinmir</v>
+        <v>Düzgündür</v>
       </c>
       <c r="T15" s="3" t="s">
         <v>13</v>
@@ -1672,13 +1675,13 @@
         <f t="shared" si="4"/>
         <v>Düzgündür</v>
       </c>
-      <c r="Q16" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="R16" s="1"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="S16" s="6" t="str">
         <f t="shared" si="5"/>
-        <v>Bilinmir</v>
+        <v>Düzgündür</v>
       </c>
       <c r="T16" s="3" t="s">
         <v>13</v>
@@ -1733,13 +1736,13 @@
         <f t="shared" si="4"/>
         <v>Düzgündür</v>
       </c>
-      <c r="Q17" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="R17" s="1"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="S17" s="6" t="str">
         <f t="shared" si="5"/>
-        <v>Bilinmir</v>
+        <v>Düzgündür</v>
       </c>
       <c r="T17" s="3" t="s">
         <v>13</v>
@@ -1792,13 +1795,13 @@
         <f t="shared" si="4"/>
         <v>Bilinmir</v>
       </c>
-      <c r="Q18" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="R18" s="1"/>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="S18" s="6" t="str">
         <f t="shared" si="5"/>
-        <v>Bilinmir</v>
+        <v>Düzgündür</v>
       </c>
       <c r="T18" s="3" t="s">
         <v>13</v>
@@ -1853,13 +1856,13 @@
         <f t="shared" si="4"/>
         <v>Düzgündür</v>
       </c>
-      <c r="Q19" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="R19" s="1"/>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="S19" s="6" t="str">
         <f t="shared" si="5"/>
-        <v>Bilinmir</v>
+        <v>Düzgündür</v>
       </c>
       <c r="T19" s="3" t="s">
         <v>13</v>
@@ -1914,13 +1917,13 @@
         <f t="shared" si="4"/>
         <v>Düzgündür</v>
       </c>
-      <c r="Q20" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="R20" s="1"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="S20" s="6" t="str">
         <f t="shared" si="5"/>
-        <v>Bilinmir</v>
+        <v>Düzgündür</v>
       </c>
       <c r="T20" s="3" t="s">
         <v>13</v>
@@ -1975,13 +1978,13 @@
         <f t="shared" si="4"/>
         <v>Düzgündür</v>
       </c>
-      <c r="Q21" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="R21" s="1"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="S21" s="6" t="str">
         <f t="shared" si="5"/>
-        <v>Bilinmir</v>
+        <v>Düzgündür</v>
       </c>
       <c r="T21" s="3" t="s">
         <v>13</v>
@@ -2036,13 +2039,13 @@
         <f t="shared" si="4"/>
         <v>Düzgündür</v>
       </c>
-      <c r="Q22" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="R22" s="1"/>
+      <c r="Q22" s="3"/>
+      <c r="R22" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="S22" s="6" t="str">
         <f t="shared" si="5"/>
-        <v>Bilinmir</v>
+        <v>Düzgündür</v>
       </c>
       <c r="T22" s="3" t="s">
         <v>13</v>
@@ -2097,13 +2100,13 @@
         <f t="shared" si="4"/>
         <v>Bilinmir</v>
       </c>
-      <c r="Q23" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="R23" s="1"/>
+      <c r="Q23" s="3"/>
+      <c r="R23" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="S23" s="6" t="str">
         <f t="shared" si="5"/>
-        <v>Bilinmir</v>
+        <v>Düzgündür</v>
       </c>
       <c r="T23" s="3" t="s">
         <v>13</v>
@@ -2158,13 +2161,13 @@
         <f t="shared" si="4"/>
         <v>Düzgündür</v>
       </c>
-      <c r="Q24" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="R24" s="1"/>
+      <c r="Q24" s="3"/>
+      <c r="R24" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="S24" s="6" t="str">
         <f t="shared" si="5"/>
-        <v>Bilinmir</v>
+        <v>Düzgündür</v>
       </c>
       <c r="T24" s="3" t="s">
         <v>13</v>
@@ -2219,13 +2222,13 @@
         <f t="shared" si="4"/>
         <v>Düzgündür</v>
       </c>
-      <c r="Q25" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="R25" s="1"/>
+      <c r="Q25" s="3"/>
+      <c r="R25" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="S25" s="6" t="str">
         <f t="shared" si="5"/>
-        <v>Bilinmir</v>
+        <v>Düzgündür</v>
       </c>
       <c r="T25" s="3" t="s">
         <v>13</v>
@@ -2282,13 +2285,13 @@
         <f t="shared" si="4"/>
         <v>Düzgündür</v>
       </c>
-      <c r="Q26" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="R26" s="1"/>
+      <c r="Q26" s="3"/>
+      <c r="R26" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="S26" s="6" t="str">
         <f t="shared" si="5"/>
-        <v>Bilinmir</v>
+        <v>Düzgündür</v>
       </c>
       <c r="T26" s="3" t="s">
         <v>13</v>
@@ -2345,9 +2348,7 @@
         <f t="shared" si="4"/>
         <v>Düzgündür</v>
       </c>
-      <c r="Q27" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="Q27" s="3"/>
       <c r="R27" s="1" t="s">
         <v>13</v>
       </c>
@@ -2410,13 +2411,13 @@
         <f t="shared" si="4"/>
         <v>Düzgündür</v>
       </c>
-      <c r="Q28" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="R28" s="1"/>
+      <c r="Q28" s="3"/>
+      <c r="R28" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="S28" s="6" t="str">
         <f t="shared" si="5"/>
-        <v>Bilinmir</v>
+        <v>Düzgündür</v>
       </c>
       <c r="T28" s="3" t="s">
         <v>13</v>
@@ -2471,9 +2472,7 @@
         <f t="shared" si="4"/>
         <v>Düzgündür</v>
       </c>
-      <c r="Q29" s="8" t="s">
-        <v>13</v>
-      </c>
+      <c r="Q29" s="8"/>
       <c r="R29" s="9" t="s">
         <v>13</v>
       </c>

</xml_diff>